<commit_message>
Gitignore and control arms progress
</commit_message>
<xml_diff>
--- a/200 - Chassis/210 - Control Arms/Control Arm Naming Guide.xlsx
+++ b/200 - Chassis/210 - Control Arms/Control Arm Naming Guide.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajkof\Documents\Wisconsin Racing\svn\222\Solidworks\200 - Chassis\210 - Control Arms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajkof\Documents\Wisconsin Racing\git\CAD\active-cad\200 - Chassis\210 - Control Arms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BBC8BD5-1FAA-4E3E-8EB5-2CDAD7AE3D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{525F41FF-78E8-422C-8CDE-62A48C5527B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1995" windowWidth="29040" windowHeight="17640" xr2:uid="{42610CB4-049C-45A7-9990-C2DEF4AC588F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{42610CB4-049C-45A7-9990-C2DEF4AC588F}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts" sheetId="1" r:id="rId1"/>
@@ -205,9 +205,6 @@
     <t>Carry Over</t>
   </si>
   <si>
-    <t>Re-Run FEA for rear lower</t>
-  </si>
-  <si>
     <t>Needs Design</t>
   </si>
   <si>
@@ -230,6 +227,9 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>Carry Over - FEA OK</t>
   </si>
 </sst>
 </file>
@@ -639,7 +639,7 @@
   <dimension ref="A1:T30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -716,7 +716,7 @@
         <v>5</v>
       </c>
       <c r="I5" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
@@ -756,7 +756,7 @@
         <v>50</v>
       </c>
       <c r="I7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
@@ -785,7 +785,7 @@
         <v>34</v>
       </c>
       <c r="I10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
@@ -805,7 +805,7 @@
         <v>35</v>
       </c>
       <c r="I11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
@@ -825,7 +825,7 @@
         <v>36</v>
       </c>
       <c r="I12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
@@ -845,7 +845,7 @@
         <v>37</v>
       </c>
       <c r="I13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
@@ -865,7 +865,7 @@
         <v>46</v>
       </c>
       <c r="I14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
@@ -885,16 +885,16 @@
         <v>47</v>
       </c>
       <c r="I15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L15" t="s">
+        <v>60</v>
+      </c>
+      <c r="P15" t="s">
         <v>61</v>
       </c>
-      <c r="P15" t="s">
+      <c r="T15" t="s">
         <v>62</v>
-      </c>
-      <c r="T15" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
@@ -914,7 +914,7 @@
         <v>45</v>
       </c>
       <c r="I16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -934,7 +934,7 @@
         <v>48</v>
       </c>
       <c r="I17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -954,7 +954,7 @@
         <v>49</v>
       </c>
       <c r="I18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -971,7 +971,7 @@
         <v>20</v>
       </c>
       <c r="I19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -1003,7 +1003,7 @@
         <v>38</v>
       </c>
       <c r="I23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
@@ -1023,7 +1023,7 @@
         <v>39</v>
       </c>
       <c r="I24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
@@ -1043,7 +1043,7 @@
         <v>40</v>
       </c>
       <c r="I25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
@@ -1063,7 +1063,7 @@
         <v>41</v>
       </c>
       <c r="I26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
@@ -1083,7 +1083,7 @@
         <v>42</v>
       </c>
       <c r="I27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
@@ -1103,7 +1103,7 @@
         <v>43</v>
       </c>
       <c r="I28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
@@ -1123,7 +1123,7 @@
         <v>44</v>
       </c>
       <c r="I29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
@@ -1261,7 +1261,7 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="161.4" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update Control Arm Naming Guide.xlsx
</commit_message>
<xml_diff>
--- a/200 - Chassis/210 - Control Arms/Control Arm Naming Guide.xlsx
+++ b/200 - Chassis/210 - Control Arms/Control Arm Naming Guide.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajkof\Documents\Wisconsin Racing\git\CAD\active-cad\200 - Chassis\210 - Control Arms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{525F41FF-78E8-422C-8CDE-62A48C5527B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{891C82E6-6120-4AC7-9DAD-AD4B4A283474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{42610CB4-049C-45A7-9990-C2DEF4AC588F}"/>
+    <workbookView xWindow="13728" yWindow="1092" windowWidth="17280" windowHeight="8964" xr2:uid="{42610CB4-049C-45A7-9990-C2DEF4AC588F}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="66">
   <si>
     <t>Description</t>
   </si>
@@ -230,6 +230,9 @@
   </si>
   <si>
     <t>Carry Over - FEA OK</t>
+  </si>
+  <si>
+    <t>QTY</t>
   </si>
 </sst>
 </file>
@@ -638,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C3B9C7F-7B97-4B66-9CA8-9719EFF74CB4}">
   <dimension ref="A1:T30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -670,6 +673,9 @@
       <c r="G1" t="s">
         <v>1</v>
       </c>
+      <c r="H1" t="s">
+        <v>65</v>
+      </c>
       <c r="I1" t="s">
         <v>54</v>
       </c>
@@ -695,6 +701,9 @@
       <c r="G4" t="s">
         <v>3</v>
       </c>
+      <c r="H4">
+        <v>24</v>
+      </c>
       <c r="I4" t="s">
         <v>55</v>
       </c>
@@ -784,6 +793,9 @@
       <c r="G10" t="s">
         <v>34</v>
       </c>
+      <c r="H10">
+        <v>3</v>
+      </c>
       <c r="I10" t="s">
         <v>63</v>
       </c>
@@ -803,6 +815,9 @@
       </c>
       <c r="G11" t="s">
         <v>35</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
       </c>
       <c r="I11" t="s">
         <v>63</v>
@@ -824,6 +839,9 @@
       <c r="G12" t="s">
         <v>36</v>
       </c>
+      <c r="H12">
+        <v>3</v>
+      </c>
       <c r="I12" t="s">
         <v>63</v>
       </c>
@@ -844,6 +862,9 @@
       <c r="G13" t="s">
         <v>37</v>
       </c>
+      <c r="H13">
+        <v>3</v>
+      </c>
       <c r="I13" t="s">
         <v>63</v>
       </c>
@@ -864,6 +885,9 @@
       <c r="G14" t="s">
         <v>46</v>
       </c>
+      <c r="H14">
+        <v>3</v>
+      </c>
       <c r="I14" t="s">
         <v>63</v>
       </c>
@@ -884,6 +908,9 @@
       <c r="G15" t="s">
         <v>47</v>
       </c>
+      <c r="H15">
+        <v>3</v>
+      </c>
       <c r="I15" t="s">
         <v>58</v>
       </c>
@@ -913,6 +940,9 @@
       <c r="G16" t="s">
         <v>45</v>
       </c>
+      <c r="H16">
+        <v>6</v>
+      </c>
       <c r="I16" t="s">
         <v>63</v>
       </c>
@@ -1002,6 +1032,9 @@
       <c r="G23" t="s">
         <v>38</v>
       </c>
+      <c r="H23">
+        <v>3</v>
+      </c>
       <c r="I23" t="s">
         <v>63</v>
       </c>
@@ -1021,6 +1054,9 @@
       </c>
       <c r="G24" t="s">
         <v>39</v>
+      </c>
+      <c r="H24">
+        <v>3</v>
       </c>
       <c r="I24" t="s">
         <v>63</v>
@@ -1042,6 +1078,9 @@
       <c r="G25" t="s">
         <v>40</v>
       </c>
+      <c r="H25">
+        <v>3</v>
+      </c>
       <c r="I25" t="s">
         <v>63</v>
       </c>
@@ -1062,6 +1101,9 @@
       <c r="G26" t="s">
         <v>41</v>
       </c>
+      <c r="H26">
+        <v>3</v>
+      </c>
       <c r="I26" t="s">
         <v>63</v>
       </c>
@@ -1082,6 +1124,9 @@
       <c r="G27" t="s">
         <v>42</v>
       </c>
+      <c r="H27">
+        <v>3</v>
+      </c>
       <c r="I27" t="s">
         <v>56</v>
       </c>
@@ -1102,6 +1147,9 @@
       <c r="G28" t="s">
         <v>43</v>
       </c>
+      <c r="H28">
+        <v>3</v>
+      </c>
       <c r="I28" t="s">
         <v>56</v>
       </c>
@@ -1122,6 +1170,9 @@
       <c r="G29" t="s">
         <v>44</v>
       </c>
+      <c r="H29">
+        <v>6</v>
+      </c>
       <c r="I29" t="s">
         <v>56</v>
       </c>
@@ -1141,6 +1192,9 @@
       </c>
       <c r="G30" t="s">
         <v>32</v>
+      </c>
+      <c r="H30">
+        <v>3</v>
       </c>
       <c r="I30" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
Kin update for front actuation, chassis stuff
</commit_message>
<xml_diff>
--- a/200 - Chassis/210 - Control Arms/Control Arm Naming Guide.xlsx
+++ b/200 - Chassis/210 - Control Arms/Control Arm Naming Guide.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajkof\Documents\Wisconsin Racing\git\CAD\active-cad\200 - Chassis\210 - Control Arms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{891C82E6-6120-4AC7-9DAD-AD4B4A283474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46DD259-B4E7-4C4F-9770-B0F7D7B1A213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13728" yWindow="1092" windowWidth="17280" windowHeight="8964" xr2:uid="{42610CB4-049C-45A7-9990-C2DEF4AC588F}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" xr2:uid="{42610CB4-049C-45A7-9990-C2DEF4AC588F}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="68">
   <si>
     <t>Description</t>
   </si>
@@ -211,9 +211,6 @@
     <t>Needs Design Refresh &amp; FEA Run</t>
   </si>
   <si>
-    <t>Serious FEA issues</t>
-  </si>
-  <si>
     <t>F Lower OB Reinforcing Plate</t>
   </si>
   <si>
@@ -233,6 +230,15 @@
   </si>
   <si>
     <t>QTY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">444 (Tens) Fore, 5 (Tens) Aft </t>
+  </si>
+  <si>
+    <t>271 (Tens) Fore, -130 (Comp) Aft</t>
+  </si>
+  <si>
+    <t>Recheck FEA/calc</t>
   </si>
 </sst>
 </file>
@@ -641,8 +647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C3B9C7F-7B97-4B66-9CA8-9719EFF74CB4}">
   <dimension ref="A1:T30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -674,7 +680,7 @@
         <v>1</v>
       </c>
       <c r="H1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I1" t="s">
         <v>54</v>
@@ -725,7 +731,7 @@
         <v>5</v>
       </c>
       <c r="I5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
@@ -797,7 +803,7 @@
         <v>3</v>
       </c>
       <c r="I10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
@@ -820,7 +826,7 @@
         <v>3</v>
       </c>
       <c r="I11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
@@ -843,7 +849,7 @@
         <v>3</v>
       </c>
       <c r="I12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
@@ -866,7 +872,7 @@
         <v>3</v>
       </c>
       <c r="I13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
@@ -889,7 +895,16 @@
         <v>3</v>
       </c>
       <c r="I14" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="L14" t="s">
+        <v>65</v>
+      </c>
+      <c r="P14" t="s">
+        <v>66</v>
+      </c>
+      <c r="T14" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
@@ -912,16 +927,16 @@
         <v>3</v>
       </c>
       <c r="I15" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="L15" t="s">
+        <v>59</v>
+      </c>
+      <c r="P15" t="s">
         <v>60</v>
       </c>
-      <c r="P15" t="s">
+      <c r="T15" t="s">
         <v>61</v>
-      </c>
-      <c r="T15" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
@@ -944,7 +959,7 @@
         <v>6</v>
       </c>
       <c r="I16" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -1036,7 +1051,7 @@
         <v>3</v>
       </c>
       <c r="I23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
@@ -1059,7 +1074,7 @@
         <v>3</v>
       </c>
       <c r="I24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
@@ -1082,7 +1097,7 @@
         <v>3</v>
       </c>
       <c r="I25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
@@ -1105,7 +1120,7 @@
         <v>3</v>
       </c>
       <c r="I26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
@@ -1315,7 +1330,7 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="161.4" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Minor kin change and front suspension outboard chassis parts finished
</commit_message>
<xml_diff>
--- a/200 - Chassis/210 - Control Arms/Control Arm Naming Guide.xlsx
+++ b/200 - Chassis/210 - Control Arms/Control Arm Naming Guide.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajkof\Documents\Wisconsin Racing\git\CAD\active-cad\200 - Chassis\210 - Control Arms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46DD259-B4E7-4C4F-9770-B0F7D7B1A213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E4B79D-85FC-4A82-BE3C-273C6C3A7136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" xr2:uid="{42610CB4-049C-45A7-9990-C2DEF4AC588F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{42610CB4-049C-45A7-9990-C2DEF4AC588F}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="67">
   <si>
     <t>Description</t>
   </si>
@@ -236,9 +236,6 @@
   </si>
   <si>
     <t>271 (Tens) Fore, -130 (Comp) Aft</t>
-  </si>
-  <si>
-    <t>Recheck FEA/calc</t>
   </si>
 </sst>
 </file>
@@ -647,8 +644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C3B9C7F-7B97-4B66-9CA8-9719EFF74CB4}">
   <dimension ref="A1:T30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -886,7 +883,7 @@
         <v>22</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="G14" t="s">
         <v>46</v>
@@ -959,7 +956,7 @@
         <v>6</v>
       </c>
       <c r="I16" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Chassis parts and dxfs
</commit_message>
<xml_diff>
--- a/200 - Chassis/210 - Control Arms/Control Arm Naming Guide.xlsx
+++ b/200 - Chassis/210 - Control Arms/Control Arm Naming Guide.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajkof\Documents\Wisconsin Racing\git\CAD\active-cad\200 - Chassis\210 - Control Arms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{526D308C-C893-43CA-8EE4-B70CFA007050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FD6D94-CB20-489E-956B-29DB946C5ACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11556" yWindow="120" windowWidth="21600" windowHeight="11208" xr2:uid="{42610CB4-049C-45A7-9990-C2DEF4AC588F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{42610CB4-049C-45A7-9990-C2DEF4AC588F}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts" sheetId="1" r:id="rId1"/>
     <sheet name="Lug Calc Screenshots" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -657,20 +656,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C3B9C7F-7B97-4B66-9CA8-9719EFF74CB4}">
   <dimension ref="A1:T30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="3.42578125" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.6640625" customWidth="1"/>
+    <col min="6" max="6" width="3.44140625" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
@@ -696,12 +695,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B4" s="1">
         <v>1</v>
       </c>
@@ -724,7 +723,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>3</v>
       </c>
@@ -744,7 +743,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>5</v>
       </c>
@@ -764,7 +763,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <v>7</v>
       </c>
@@ -784,16 +783,16 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B10" s="1">
         <v>1</v>
       </c>
@@ -816,7 +815,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B11" s="1">
         <v>3</v>
       </c>
@@ -839,7 +838,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B12" s="1">
         <v>5</v>
       </c>
@@ -862,7 +861,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <v>7</v>
       </c>
@@ -885,7 +884,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B14" s="1">
         <v>9</v>
       </c>
@@ -917,7 +916,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B15" s="1">
         <v>11</v>
       </c>
@@ -949,7 +948,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B16" s="1">
         <v>13</v>
       </c>
@@ -972,7 +971,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B17" s="1">
         <v>15</v>
       </c>
@@ -992,7 +991,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B18" s="1">
         <v>17</v>
       </c>
@@ -1012,7 +1011,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B19" s="1">
         <v>19</v>
       </c>
@@ -1029,19 +1028,19 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B23" s="1">
         <v>1</v>
       </c>
@@ -1064,7 +1063,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B24" s="1">
         <v>3</v>
       </c>
@@ -1087,7 +1086,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B25" s="1">
         <v>5</v>
       </c>
@@ -1110,7 +1109,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B26" s="1">
         <v>7</v>
       </c>
@@ -1133,7 +1132,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B27" s="1">
         <v>9</v>
       </c>
@@ -1153,7 +1152,7 @@
         <v>3</v>
       </c>
       <c r="I27" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="L27" t="s">
         <v>70</v>
@@ -1162,7 +1161,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B28" s="1">
         <v>11</v>
       </c>
@@ -1191,7 +1190,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B29" s="1">
         <v>13</v>
       </c>
@@ -1211,10 +1210,10 @@
         <v>6</v>
       </c>
       <c r="I29" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B30" s="1">
         <v>15</v>
       </c>
@@ -1251,14 +1250,14 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -1266,7 +1265,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B4" s="1">
         <v>3</v>
       </c>
@@ -1274,7 +1273,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>5</v>
       </c>
@@ -1282,7 +1281,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>7</v>
       </c>
@@ -1290,16 +1289,16 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" s="1">
         <v>1</v>
       </c>
@@ -1307,7 +1306,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" s="1">
         <v>3</v>
       </c>
@@ -1315,7 +1314,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" s="1">
         <v>5</v>
       </c>
@@ -1323,7 +1322,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" s="1">
         <v>7</v>
       </c>
@@ -1331,7 +1330,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <v>9</v>
       </c>
@@ -1339,7 +1338,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" s="1">
         <v>11</v>
       </c>
@@ -1347,7 +1346,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" s="1">
         <v>13</v>
       </c>
@@ -1355,7 +1354,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="161.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="161.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="1">
         <v>15</v>
       </c>
@@ -1363,7 +1362,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B17" s="1">
         <v>17</v>
       </c>
@@ -1371,7 +1370,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B18" s="1">
         <v>19</v>
       </c>
@@ -1379,7 +1378,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B19" s="1">
         <v>21</v>
       </c>
@@ -1387,16 +1386,16 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B22" s="1">
         <v>1</v>
       </c>
@@ -1404,7 +1403,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B23" s="1">
         <v>3</v>
       </c>
@@ -1412,7 +1411,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B24" s="1">
         <v>5</v>
       </c>
@@ -1420,7 +1419,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B25" s="1">
         <v>7</v>
       </c>
@@ -1428,7 +1427,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B26" s="1">
         <v>9</v>
       </c>
@@ -1436,7 +1435,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B27" s="1">
         <v>11</v>
       </c>
@@ -1444,7 +1443,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B28" s="1">
         <v>13</v>
       </c>
@@ -1452,7 +1451,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B29" s="1">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Clevis and shim updates
</commit_message>
<xml_diff>
--- a/200 - Chassis/210 - Control Arms/Control Arm Naming Guide.xlsx
+++ b/200 - Chassis/210 - Control Arms/Control Arm Naming Guide.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajkof\Documents\Wisconsin Racing\git\CAD\active-cad\200 - Chassis\210 - Control Arms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajkof\Documents\Wisconsin Racing\git\active-cad\200 - Chassis\210 - Control Arms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8855D7-DB50-4E12-9BBB-0B455F1B2212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D0D4C9-07EA-4C4D-BAE7-C743E657A3BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16140" yWindow="2568" windowWidth="6900" windowHeight="5736" xr2:uid="{42610CB4-049C-45A7-9990-C2DEF4AC588F}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{42610CB4-049C-45A7-9990-C2DEF4AC588F}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="74">
   <si>
     <t>Description</t>
   </si>
@@ -223,9 +223,6 @@
     <t>Done</t>
   </si>
   <si>
-    <t>Carry Over - FEA OK</t>
-  </si>
-  <si>
     <t>QTY</t>
   </si>
   <si>
@@ -248,6 +245,18 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>0.3125 x 4</t>
+  </si>
+  <si>
+    <t>0.125 x 20</t>
+  </si>
+  <si>
+    <t>0.063 x 8</t>
+  </si>
+  <si>
+    <t>0.032 x 8</t>
   </si>
 </sst>
 </file>
@@ -656,8 +665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C3B9C7F-7B97-4B66-9CA8-9719EFF74CB4}">
   <dimension ref="A1:T30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -667,6 +676,8 @@
     <col min="5" max="5" width="4.6640625" customWidth="1"/>
     <col min="6" max="6" width="3.44140625" customWidth="1"/>
     <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.44140625" customWidth="1"/>
+    <col min="13" max="13" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
@@ -689,10 +700,10 @@
         <v>1</v>
       </c>
       <c r="H1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
@@ -731,7 +742,7 @@
         <v>4</v>
       </c>
       <c r="D5">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
         <v>20</v>
@@ -740,7 +751,7 @@
         <v>5</v>
       </c>
       <c r="I5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
@@ -751,7 +762,7 @@
         <v>6</v>
       </c>
       <c r="D6">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
         <v>20</v>
@@ -760,7 +771,19 @@
         <v>7</v>
       </c>
       <c r="I6" t="s">
-        <v>54</v>
+        <v>61</v>
+      </c>
+      <c r="L6" t="s">
+        <v>70</v>
+      </c>
+      <c r="M6" t="s">
+        <v>71</v>
+      </c>
+      <c r="N6" t="s">
+        <v>72</v>
+      </c>
+      <c r="O6" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
@@ -907,10 +930,10 @@
         <v>61</v>
       </c>
       <c r="L14" t="s">
+        <v>63</v>
+      </c>
+      <c r="P14" t="s">
         <v>64</v>
-      </c>
-      <c r="P14" t="s">
-        <v>65</v>
       </c>
       <c r="T14" t="s">
         <v>60</v>
@@ -1155,10 +1178,10 @@
         <v>61</v>
       </c>
       <c r="L27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
@@ -1184,10 +1207,10 @@
         <v>61</v>
       </c>
       <c r="L28" t="s">
+        <v>65</v>
+      </c>
+      <c r="P28" t="s">
         <v>66</v>
-      </c>
-      <c r="P28" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">

</xml_diff>